<commit_message>
Add báo cáo tham khảo BA
</commit_message>
<xml_diff>
--- a/Tracking.xlsx
+++ b/Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DUE\COURSES\MIS4002. Thực tập tốt nghiệp\07.2021-2022.2\ThucTapTN_2021_2022_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2794C98B-8537-470D-8A92-065FF3D648F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF95D7A-B8A7-4585-9C44-D9C57C1164B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
   <si>
     <t>STT</t>
   </si>
@@ -493,6 +493,39 @@
   </si>
   <si>
     <t>Cần mô tả chi tiết các UC mà em sẽ test</t>
+  </si>
+  <si>
+    <t>vắng, báo cáo qua IB</t>
+  </si>
+  <si>
+    <t>xong PT, đã push git</t>
+  </si>
+  <si>
+    <t>xong PT, đã push git
+viết lại tổng quan: kiến trúc/component model --&gt; bức tranh tổng thể hệ thống</t>
+  </si>
+  <si>
+    <t>đổi sang dự án 2, làm lại báo cáo: tập trung vào PT</t>
+  </si>
+  <si>
+    <t>Test toàn bộ manage courses
+Phân tích lại manage courses</t>
+  </si>
+  <si>
+    <t>viết lại chương 5</t>
+  </si>
+  <si>
+    <t>Chuyển sang làm test
+Viết xong công cụ bird eat bugs
+PHân tích hệ thống</t>
+  </si>
+  <si>
+    <t>Đẩy nhanh tiến độ frontend
+Thêm: báo cáo cho các roles
+Thêm: "phản ánh sai"</t>
+  </si>
+  <si>
+    <t>viết lại phân tích nghiệp vụ thực tế</t>
   </si>
 </sst>
 </file>
@@ -763,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -796,7 +829,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -818,9 +850,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -880,6 +909,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -896,15 +929,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,9 +1162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1142,10 +1181,11 @@
     <col min="10" max="10" width="20.25" customWidth="1"/>
     <col min="12" max="12" width="49.625" customWidth="1"/>
     <col min="13" max="13" width="46.125" customWidth="1"/>
-    <col min="14" max="14" width="23.875" style="51" customWidth="1"/>
+    <col min="14" max="14" width="23.875" style="49" customWidth="1"/>
     <col min="15" max="15" width="13.25" customWidth="1"/>
     <col min="16" max="16" width="19" customWidth="1"/>
-    <col min="17" max="26" width="7.625" customWidth="1"/>
+    <col min="17" max="17" width="48" customWidth="1"/>
+    <col min="18" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="75">
@@ -1188,19 +1228,21 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
+      <c r="Q1" s="31">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
@@ -1243,74 +1285,78 @@
       <c r="L2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
+      <c r="Q2" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
     </row>
-    <row r="3" spans="1:26" s="45" customFormat="1">
-      <c r="A3" s="38">
+    <row r="3" spans="1:26" s="43" customFormat="1">
+      <c r="A3" s="36">
         <v>3</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42" t="s">
+      <c r="K3" s="39"/>
+      <c r="L3" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="O3" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
+      <c r="Q3" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" hidden="1">
       <c r="A4" s="6">
         <v>4</v>
       </c>
@@ -1337,66 +1383,68 @@
       <c r="J4" s="9"/>
       <c r="K4" s="8"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="49"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
     </row>
-    <row r="5" spans="1:26" s="21" customFormat="1" ht="29.25">
-      <c r="A5" s="17">
+    <row r="5" spans="1:26" s="43" customFormat="1" ht="43.5">
+      <c r="A5" s="36">
         <v>5</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="22" t="s">
+      <c r="K5" s="36"/>
+      <c r="L5" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33" t="s">
+      <c r="O5" s="42"/>
+      <c r="P5" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
+      <c r="Q5" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
     </row>
     <row r="6" spans="1:26" ht="43.5">
       <c r="A6" s="6">
@@ -1433,68 +1481,70 @@
       <c r="L6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="N6" s="67" t="s">
+      <c r="N6" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="O6" s="34"/>
-      <c r="P6" s="74" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
     </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="29.25">
-      <c r="A7" s="38">
+    <row r="7" spans="1:26" s="43" customFormat="1" ht="57.75">
+      <c r="A7" s="36">
         <v>7</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="39" t="s">
+      <c r="I7" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="46" t="s">
+      <c r="K7" s="39"/>
+      <c r="L7" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="M7" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="N7" s="48" t="s">
+      <c r="N7" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
     </row>
     <row r="8" spans="1:26" s="21" customFormat="1">
       <c r="A8" s="17">
@@ -1522,7 +1572,7 @@
       <c r="I8" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="22" t="s">
         <v>59</v>
       </c>
       <c r="K8" s="20"/>
@@ -1535,208 +1585,216 @@
       <c r="N8" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="75" t="s">
+      <c r="O8" s="32"/>
+      <c r="P8" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
+      <c r="Q8" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
     </row>
-    <row r="9" spans="1:26" s="21" customFormat="1">
-      <c r="A9" s="24">
+    <row r="9" spans="1:26" s="21" customFormat="1" ht="36" customHeight="1">
+      <c r="A9" s="23">
         <v>18</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="24">
         <v>44682</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="22" t="s">
         <v>63</v>
       </c>
       <c r="K9" s="20"/>
       <c r="L9" s="69"/>
       <c r="M9" s="71"/>
       <c r="N9" s="73"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33"/>
-      <c r="T9" s="33"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
     </row>
-    <row r="10" spans="1:26" s="45" customFormat="1">
-      <c r="A10" s="38">
+    <row r="10" spans="1:26" s="43" customFormat="1" ht="29.25">
+      <c r="A10" s="36">
         <v>9</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41" t="s">
+      <c r="K10" s="39"/>
+      <c r="L10" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="M10" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="48" t="s">
+      <c r="N10" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="O10" s="44" t="s">
+      <c r="O10" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="P10" s="44" t="s">
+      <c r="P10" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
+      <c r="Q10" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
     </row>
-    <row r="11" spans="1:26" s="60" customFormat="1" ht="29.25">
-      <c r="A11" s="52">
+    <row r="11" spans="1:26" s="58" customFormat="1" ht="29.25">
+      <c r="A11" s="50">
         <v>10</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="53" t="s">
+      <c r="I11" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="54" t="s">
+      <c r="J11" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="55"/>
-      <c r="L11" s="56" t="s">
+      <c r="K11" s="53"/>
+      <c r="L11" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="M11" s="57" t="s">
+      <c r="M11" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="N11" s="58" t="s">
+      <c r="N11" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="O11" s="59" t="s">
+      <c r="O11" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="59"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
     </row>
-    <row r="12" spans="1:26" s="45" customFormat="1">
-      <c r="A12" s="38">
+    <row r="12" spans="1:26" s="43" customFormat="1" ht="29.25">
+      <c r="A12" s="36">
         <v>11</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="40" t="s">
+      <c r="J12" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="K12" s="41"/>
-      <c r="L12" s="47" t="s">
+      <c r="K12" s="39"/>
+      <c r="L12" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="M12" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="N12" s="48" t="s">
+      <c r="N12" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="O12" s="44" t="s">
+      <c r="O12" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="P12" s="44" t="s">
+      <c r="P12" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="44"/>
+      <c r="Q12" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
     </row>
     <row r="13" spans="1:26" hidden="1">
       <c r="A13" s="11">
@@ -1761,14 +1819,14 @@
       <c r="J13" s="13"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="15"/>
@@ -1811,20 +1869,22 @@
       <c r="L14" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="M14" s="26" t="s">
+      <c r="M14" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="O14" s="36" t="s">
+      <c r="O14" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="33"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
     </row>
     <row r="15" spans="1:26" ht="86.25">
       <c r="A15" s="6">
@@ -1863,22 +1923,22 @@
       <c r="L15" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="M15" s="27" t="s">
+      <c r="M15" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="N15" s="67" t="s">
+      <c r="N15" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="O15" s="34"/>
-      <c r="P15" s="77" t="s">
+      <c r="O15" s="33"/>
+      <c r="P15" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
     </row>
-    <row r="16" spans="1:26" s="21" customFormat="1">
+    <row r="16" spans="1:26" s="21" customFormat="1" hidden="1">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -1913,70 +1973,72 @@
       <c r="L16" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="N16" s="36" t="s">
+      <c r="N16" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
     </row>
-    <row r="17" spans="1:20" s="45" customFormat="1" ht="42.75">
-      <c r="A17" s="62">
+    <row r="17" spans="1:20" s="43" customFormat="1" ht="42.75">
+      <c r="A17" s="60">
         <v>16</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="62" t="s">
+      <c r="G17" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="62" t="s">
+      <c r="H17" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="I17" s="63" t="s">
+      <c r="I17" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="K17" s="62" t="s">
+      <c r="K17" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="L17" s="65" t="s">
+      <c r="L17" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="M17" s="66" t="s">
+      <c r="M17" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="N17" s="48" t="s">
+      <c r="N17" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44" t="s">
+      <c r="O17" s="42"/>
+      <c r="P17" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
+      <c r="Q17" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1">
       <c r="C19" s="5">
@@ -2964,11 +3026,12 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Review báo cáo Nhi
</commit_message>
<xml_diff>
--- a/Tracking.xlsx
+++ b/Tracking.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DUE\COURSES\MIS4002. Thực tập tốt nghiệp\07.2021-2022.2\ThucTapTN_2021_2022_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEMP\ThucTapTN_2021_2022_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF95D7A-B8A7-4585-9C44-D9C57C1164B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A67E7-A39E-4B6E-BD53-7CB4F04CA0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7midSKLJmL0M3KR4ORSBe4VAgbHq2A=="/>
     </ext>
@@ -535,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,6 +921,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -934,13 +949,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1164,31 +1172,31 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="31.25" customWidth="1"/>
-    <col min="6" max="6" width="19.875" customWidth="1"/>
-    <col min="7" max="7" width="7.625" customWidth="1"/>
-    <col min="8" max="8" width="13.875" customWidth="1"/>
-    <col min="9" max="9" width="9.375" customWidth="1"/>
-    <col min="10" max="10" width="20.25" customWidth="1"/>
-    <col min="12" max="12" width="49.625" customWidth="1"/>
-    <col min="13" max="13" width="46.125" customWidth="1"/>
-    <col min="14" max="14" width="23.875" style="49" customWidth="1"/>
-    <col min="15" max="15" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" customWidth="1"/>
+    <col min="5" max="5" width="31.19921875" customWidth="1"/>
+    <col min="6" max="6" width="19.8984375" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" customWidth="1"/>
+    <col min="8" max="8" width="13.8984375" customWidth="1"/>
+    <col min="9" max="9" width="9.3984375" customWidth="1"/>
+    <col min="10" max="10" width="20.19921875" customWidth="1"/>
+    <col min="12" max="12" width="49.59765625" customWidth="1"/>
+    <col min="13" max="13" width="46.09765625" customWidth="1"/>
+    <col min="14" max="14" width="23.8984375" style="49" customWidth="1"/>
+    <col min="15" max="15" width="13.19921875" customWidth="1"/>
     <col min="16" max="16" width="19" customWidth="1"/>
     <col min="17" max="17" width="48" customWidth="1"/>
-    <col min="18" max="26" width="7.625" customWidth="1"/>
+    <col min="18" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="75">
+    <row r="1" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1258,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" s="21" customFormat="1" ht="29.25">
+    <row r="2" spans="1:26" s="21" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>2</v>
       </c>
@@ -1302,7 +1310,7 @@
       <c r="S2" s="32"/>
       <c r="T2" s="32"/>
     </row>
-    <row r="3" spans="1:26" s="43" customFormat="1">
+    <row r="3" spans="1:26" s="43" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="36">
         <v>3</v>
       </c>
@@ -1356,7 +1364,7 @@
       <c r="S3" s="42"/>
       <c r="T3" s="42"/>
     </row>
-    <row r="4" spans="1:26" hidden="1">
+    <row r="4" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>4</v>
       </c>
@@ -1394,7 +1402,7 @@
       <c r="S4" s="33"/>
       <c r="T4" s="33"/>
     </row>
-    <row r="5" spans="1:26" s="43" customFormat="1" ht="43.5">
+    <row r="5" spans="1:26" s="43" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A5" s="36">
         <v>5</v>
       </c>
@@ -1426,10 +1434,10 @@
         <v>41</v>
       </c>
       <c r="K5" s="36"/>
-      <c r="L5" s="77" t="s">
+      <c r="L5" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="78" t="s">
+      <c r="M5" s="70" t="s">
         <v>117</v>
       </c>
       <c r="N5" s="46" t="s">
@@ -1446,7 +1454,7 @@
       <c r="S5" s="42"/>
       <c r="T5" s="42"/>
     </row>
-    <row r="6" spans="1:26" ht="43.5">
+    <row r="6" spans="1:26" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>6</v>
       </c>
@@ -1496,7 +1504,7 @@
       <c r="S6" s="33"/>
       <c r="T6" s="33"/>
     </row>
-    <row r="7" spans="1:26" s="43" customFormat="1" ht="57.75">
+    <row r="7" spans="1:26" s="43" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="36">
         <v>7</v>
       </c>
@@ -1546,7 +1554,7 @@
       <c r="S7" s="42"/>
       <c r="T7" s="42"/>
     </row>
-    <row r="8" spans="1:26" s="21" customFormat="1">
+    <row r="8" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>8</v>
       </c>
@@ -1576,27 +1584,27 @@
         <v>59</v>
       </c>
       <c r="K8" s="20"/>
-      <c r="L8" s="68" t="s">
+      <c r="L8" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="70" t="s">
+      <c r="M8" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="N8" s="72" t="s">
+      <c r="N8" s="75" t="s">
         <v>123</v>
       </c>
       <c r="O8" s="32"/>
-      <c r="P8" s="74" t="s">
+      <c r="P8" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="Q8" s="72" t="s">
+      <c r="Q8" s="75" t="s">
         <v>154</v>
       </c>
       <c r="R8" s="32"/>
       <c r="S8" s="32"/>
       <c r="T8" s="32"/>
     </row>
-    <row r="9" spans="1:26" s="21" customFormat="1" ht="36" customHeight="1">
+    <row r="9" spans="1:26" s="21" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>18</v>
       </c>
@@ -1626,17 +1634,17 @@
         <v>63</v>
       </c>
       <c r="K9" s="20"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="71"/>
-      <c r="N9" s="73"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="32"/>
-      <c r="P9" s="75"/>
+      <c r="P9" s="78"/>
       <c r="Q9" s="79"/>
       <c r="R9" s="32"/>
       <c r="S9" s="32"/>
       <c r="T9" s="32"/>
     </row>
-    <row r="10" spans="1:26" s="43" customFormat="1" ht="29.25">
+    <row r="10" spans="1:26" s="43" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>9</v>
       </c>
@@ -1690,7 +1698,7 @@
       <c r="S10" s="42"/>
       <c r="T10" s="42"/>
     </row>
-    <row r="11" spans="1:26" s="58" customFormat="1" ht="29.25">
+    <row r="11" spans="1:26" s="58" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A11" s="50">
         <v>10</v>
       </c>
@@ -1742,7 +1750,7 @@
       <c r="S11" s="57"/>
       <c r="T11" s="57"/>
     </row>
-    <row r="12" spans="1:26" s="43" customFormat="1" ht="29.25">
+    <row r="12" spans="1:26" s="43" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>11</v>
       </c>
@@ -1796,7 +1804,7 @@
       <c r="S12" s="42"/>
       <c r="T12" s="42"/>
     </row>
-    <row r="13" spans="1:26" hidden="1">
+    <row r="13" spans="1:26" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1834,7 +1842,7 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" s="21" customFormat="1" ht="29.25">
+    <row r="14" spans="1:26" s="21" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -1886,7 +1894,7 @@
       <c r="S14" s="32"/>
       <c r="T14" s="32"/>
     </row>
-    <row r="15" spans="1:26" ht="86.25">
+    <row r="15" spans="1:26" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1938,7 +1946,7 @@
       <c r="S15" s="33"/>
       <c r="T15" s="33"/>
     </row>
-    <row r="16" spans="1:26" s="21" customFormat="1" hidden="1">
+    <row r="16" spans="1:26" s="21" customFormat="1" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -1986,7 +1994,7 @@
       <c r="S16" s="32"/>
       <c r="T16" s="32"/>
     </row>
-    <row r="17" spans="1:20" s="43" customFormat="1" ht="42.75">
+    <row r="17" spans="1:20" s="43" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A17" s="60">
         <v>16</v>
       </c>
@@ -2033,998 +2041,998 @@
       <c r="P17" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="Q17" s="76" t="s">
+      <c r="Q17" s="68" t="s">
         <v>152</v>
       </c>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
     </row>
-    <row r="19" spans="1:20" ht="15.75" customHeight="1">
+    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5">
         <f>COUNTA(C2:C17)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="L8:L9"/>

</xml_diff>